<commit_message>
updated version, still need add x and y differences
</commit_message>
<xml_diff>
--- a/misc/regresia.xlsx
+++ b/misc/regresia.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17927"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18229"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\S\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\S\Projects\tracklets\misc\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9510"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9510" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Data_20120305_2" sheetId="1" r:id="rId1"/>
@@ -979,6 +979,99 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000017-0686-40A9-AB1B-F092F6352DA2}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>ParReal</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:forward val="200"/>
+            <c:backward val="20"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>(Data_20120318_2!$A$4,Data_20120318_2!$A$15,Data_20120318_2!$A$19,Data_20120318_2!$A$27)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>22.4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>64.09</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>127.3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>190.73</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>(Data_20120318_2!$B$4,Data_20120318_2!$B$15,Data_20120318_2!$B$19,Data_20120318_2!$B$27)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>283.52999999999997</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>341.2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>443.14</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>561.47</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-EE4B-4796-A72E-9D9D7783CEF3}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2655,7 +2748,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
@@ -2924,8 +3017,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="Q13" sqref="Q13"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>